<commit_message>
Adjusted stopwatch to milliseconds
</commit_message>
<xml_diff>
--- a/Project1Table.xlsx
+++ b/Project1Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\CS 3310\Projects\MatrixMultiplication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A120B7-5D47-40E4-A5FF-C6FFBFFB04C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A14BCE-2DEB-4C29-B6D3-202BB33D2136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24AADB5E-1ECB-4C15-A64E-E7825C5C0CD1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
   <si>
     <t>Brute Force O(n^3)</t>
   </si>
@@ -49,13 +49,19 @@
     <t>Size (n)</t>
   </si>
   <si>
-    <t>Time (s)</t>
-  </si>
-  <si>
     <t>Trial 2</t>
   </si>
   <si>
     <t>Trial 3</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>Trial 1</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -86,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -110,33 +116,67 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -260,7 +300,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -293,33 +333,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.8999999999999995E-6</c:v>
+                  <c:v>7.966666666666667E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7999999999999999E-6</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5199999999999999E-5</c:v>
+                  <c:v>2.6766666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.26E-4</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.0866999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>3.1476999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>7.7313E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>2.3333E-2</c:v>
+                  <c:v>0.13500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0048666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5936333333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4711999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.17956666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,7 +402,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$10</c:f>
+              <c:f>Sheet1!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -395,33 +435,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$10</c:f>
+              <c:f>Sheet1!$D$4:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.8499999999999999E-5</c:v>
+                  <c:v>1.7966666666666669E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4099999999999999E-5</c:v>
+                  <c:v>5.8233333333333331E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3199999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>2.1833E-3</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.20138E-2</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>9.0512899999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.79596440000000002</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>5.2197787</c:v>
+                  <c:v>0.46153333333333335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3883666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.411766666666665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.735933333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>795.92140000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5269.1021333333338</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -464,7 +504,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$10</c:f>
+              <c:f>Sheet1!$E$4:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -497,33 +537,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$10</c:f>
+              <c:f>Sheet1!$F$4:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.66E-5</c:v>
+                  <c:v>1.9300000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7600000000000001E-5</c:v>
+                  <c:v>8.6466666666666678E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0100000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>2.1473999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.1525000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>7.9420199999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.45597290000000001</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>3.0180007999999998</c:v>
+                  <c:v>0.50739999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0022333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.460733333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.819266666666664</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>452.45306666666664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3124.6605666666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,9 +744,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (seconds)</a:t>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Time (milliseconds)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -969,7 +1012,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1002,33 +1045,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.8999999999999995E-6</c:v>
+                  <c:v>7.966666666666667E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7999999999999999E-6</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5199999999999999E-5</c:v>
+                  <c:v>2.6766666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.26E-4</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.0866999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>3.1476999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>7.7313E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>2.3333E-2</c:v>
+                  <c:v>0.13500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0048666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5936333333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4711999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.17956666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1210,7 +1253,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time (seconds)</a:t>
+                  <a:t>Time (milliseconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1479,7 +1522,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$10</c:f>
+              <c:f>Sheet1!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1512,33 +1555,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$10</c:f>
+              <c:f>Sheet1!$D$4:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.8499999999999999E-5</c:v>
+                  <c:v>1.7966666666666669E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4099999999999999E-5</c:v>
+                  <c:v>5.8233333333333331E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3199999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>2.1833E-3</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.20138E-2</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>9.0512899999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.79596440000000002</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>5.2197787</c:v>
+                  <c:v>0.46153333333333335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3883666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.411766666666665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.735933333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>795.92140000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5269.1021333333338</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1719,8 +1762,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (seconds)</a:t>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Time (milliseconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1913,8 +1958,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Strassens O(n^log7)</a:t>
+              <a:t>Strassen's</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Algorithm O(n^log7)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1926,26 +1976,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1984,7 +2014,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$10</c:f>
+              <c:f>Sheet1!$E$4:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2017,33 +2047,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$10</c:f>
+              <c:f>Sheet1!$F$4:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.66E-5</c:v>
+                  <c:v>1.9300000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7600000000000001E-5</c:v>
+                  <c:v>8.6466666666666678E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0100000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>2.1473999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.1525000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>7.9420199999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.45597290000000001</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>3.0180007999999998</c:v>
+                  <c:v>0.50739999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0022333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.460733333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.819266666666664</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>452.45306666666664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3124.6605666666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,7 +2081,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3038-4BB4-8D7E-9BFD0958E596}"/>
+              <c16:uniqueId val="{00000006-8E77-4C78-8F60-E8E8D1E2ED4F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2121,26 +2151,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2224,9 +2234,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (seconds)</a:t>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Time (milliseconds)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2238,26 +2251,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2300,13 +2293,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
@@ -2341,30 +2327,9 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -2503,46 +2468,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -4103,540 +4028,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4665,13 +4070,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>33338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4701,16 +4106,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4739,16 +4144,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>52388</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5078,10 +4483,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="AN14" sqref="AN14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,586 +4499,812 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>8.8999999999999995E-6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.8499999999999999E-5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.66E-5</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>7.7999999999999999E-6</v>
+        <f>AVERAGE(B14, B24, B34)</f>
+        <v>7.966666666666667E-3</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>7.4099999999999999E-5</v>
+        <f>AVERAGE(D14, D24, D34)</f>
+        <v>1.7966666666666669E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>9.7600000000000001E-5</v>
+        <f>AVERAGE(F14, F24, F34)</f>
+        <v>1.9300000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>2.5199999999999999E-5</v>
+        <f>AVERAGE(B15, B25, B35)</f>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="C5" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
-        <v>4.3199999999999998E-4</v>
+        <f>AVERAGE(D15, D25, D35)</f>
+        <v>5.8233333333333331E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F5" s="2">
-        <v>5.0100000000000003E-4</v>
+        <f>AVERAGE(F15, F25, F35)</f>
+        <v>8.6466666666666678E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>1.26E-4</v>
+        <f>AVERAGE(B16, B26, B36)</f>
+        <v>2.6766666666666671E-2</v>
       </c>
       <c r="C6" s="1">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2.1833E-3</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <f>AVERAGE(D16, D26, D36)</f>
+        <v>0.46153333333333335</v>
       </c>
       <c r="E6" s="1">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.1473999999999998E-3</v>
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <f>AVERAGE(F16, F26, F36)</f>
+        <v>0.50739999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.0866999999999999E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <f>AVERAGE(B17, B27, B37)</f>
+        <v>0.13500000000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.20138E-2</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
+        <f>AVERAGE(D17, D27, D37)</f>
+        <v>2.3883666666666667</v>
       </c>
       <c r="E7" s="1">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.1525000000000001E-2</v>
+        <v>16</v>
+      </c>
+      <c r="F7" s="2">
+        <f>AVERAGE(F17, F27, F37)</f>
+        <v>2.0022333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>64</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.1476999999999998E-3</v>
+        <v>32</v>
+      </c>
+      <c r="B8" s="2">
+        <f>AVERAGE(B18, B28, B38)</f>
+        <v>1.0048666666666668</v>
       </c>
       <c r="C8" s="1">
-        <v>64</v>
-      </c>
-      <c r="D8" s="1">
-        <v>9.0512899999999993E-2</v>
+        <v>32</v>
+      </c>
+      <c r="D8" s="2">
+        <f>AVERAGE(D18, D28, D38)</f>
+        <v>12.411766666666665</v>
       </c>
       <c r="E8" s="1">
-        <v>64</v>
-      </c>
-      <c r="F8" s="1">
-        <v>7.9420199999999996E-2</v>
+        <v>32</v>
+      </c>
+      <c r="F8" s="2">
+        <f>AVERAGE(F18, F28, F38)</f>
+        <v>12.460733333333335</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>128</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7.7313E-3</v>
+        <v>64</v>
+      </c>
+      <c r="B9" s="2">
+        <f>AVERAGE(B19, B29, B39)</f>
+        <v>2.5936333333333335</v>
       </c>
       <c r="C9" s="1">
-        <v>128</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.79596440000000002</v>
+        <v>64</v>
+      </c>
+      <c r="D9" s="2">
+        <f>AVERAGE(D19, D29, D39)</f>
+        <v>90.735933333333335</v>
       </c>
       <c r="E9" s="1">
-        <v>128</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.45597290000000001</v>
+        <v>64</v>
+      </c>
+      <c r="F9" s="2">
+        <f>AVERAGE(F19, F29, F39)</f>
+        <v>80.819266666666664</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>256</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2.3333E-2</v>
+        <v>128</v>
+      </c>
+      <c r="B10" s="2">
+        <f>AVERAGE(B20, B30, B40)</f>
+        <v>8.4711999999999996</v>
       </c>
       <c r="C10" s="1">
-        <v>256</v>
-      </c>
-      <c r="D10" s="1">
-        <v>5.2197787</v>
+        <v>128</v>
+      </c>
+      <c r="D10" s="2">
+        <f>AVERAGE(D20, D30, D40)</f>
+        <v>795.92140000000006</v>
       </c>
       <c r="E10" s="1">
-        <v>256</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3.0180007999999998</v>
+        <v>128</v>
+      </c>
+      <c r="F10" s="2">
+        <f>AVERAGE(F20, F30, F40)</f>
+        <v>452.45306666666664</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="1">
+        <v>256</v>
+      </c>
+      <c r="B11" s="2">
+        <f>AVERAGE(B21, B31, B41)</f>
+        <v>23.17956666666667</v>
+      </c>
+      <c r="C11" s="1">
+        <v>256</v>
+      </c>
+      <c r="D11" s="2">
+        <f>AVERAGE(D21, D31, D41)</f>
+        <v>5269.1021333333338</v>
+      </c>
+      <c r="E11" s="1">
+        <v>256</v>
+      </c>
+      <c r="F11" s="2">
+        <f>AVERAGE(F21, F31, F41)</f>
+        <v>3124.6605666666669</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7">
-        <v>7.1999999999999997E-6</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2.5899999999999999E-5</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2.0299999999999999E-5</v>
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>4</v>
-      </c>
-      <c r="B14" s="7">
-        <v>8.6000000000000007E-6</v>
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7">
-        <v>6.1699999999999995E-5</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>4</v>
-      </c>
-      <c r="F14" s="7">
-        <v>1.022E-4</v>
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2.1600000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7">
-        <v>2.7399999999999999E-5</v>
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="C15" s="1">
-        <v>8</v>
-      </c>
-      <c r="D15" s="7">
-        <v>4.7350000000000002E-4</v>
+        <v>4</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5.45E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>8</v>
-      </c>
-      <c r="F15" s="7">
-        <v>4.9899999999999999E-4</v>
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <v>7.2800000000000004E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>16</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1.4550000000000001E-4</v>
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="C16" s="1">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6">
-        <v>2.1186E-3</v>
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.43490000000000001</v>
       </c>
       <c r="E16" s="1">
-        <v>16</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1.8753000000000001E-3</v>
+        <v>8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.49580000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>32</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1.0192000000000001E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.14599999999999999</v>
       </c>
       <c r="C17" s="1">
-        <v>32</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1.3024900000000001E-2</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.2081</v>
       </c>
       <c r="E17" s="1">
-        <v>32</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1.1669499999999999E-2</v>
+        <v>16</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.9959</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>64</v>
-      </c>
-      <c r="B18" s="6">
-        <v>2.5195999999999999E-3</v>
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0789</v>
       </c>
       <c r="C18" s="1">
-        <v>64</v>
-      </c>
-      <c r="D18" s="6">
-        <v>8.9731199999999997E-2</v>
+        <v>32</v>
+      </c>
+      <c r="D18" s="1">
+        <v>12.7027</v>
       </c>
       <c r="E18" s="1">
-        <v>64</v>
-      </c>
-      <c r="F18" s="6">
-        <v>7.9984700000000006E-2</v>
+        <v>32</v>
+      </c>
+      <c r="F18" s="1">
+        <v>12.5938</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>128</v>
-      </c>
-      <c r="B19" s="6">
-        <v>8.7881000000000001E-3</v>
+        <v>64</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.48</v>
       </c>
       <c r="C19" s="1">
-        <v>128</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.79665940000000002</v>
+        <v>64</v>
+      </c>
+      <c r="D19" s="1">
+        <v>90.325699999999998</v>
       </c>
       <c r="E19" s="1">
-        <v>128</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0.4525267</v>
+        <v>64</v>
+      </c>
+      <c r="F19" s="1">
+        <v>81.270499999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>256</v>
-      </c>
-      <c r="B20" s="6">
-        <v>2.31535E-2</v>
+        <v>128</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.4277999999999995</v>
       </c>
       <c r="C20" s="1">
-        <v>256</v>
-      </c>
-      <c r="D20" s="6">
-        <v>5.1952167999999999</v>
+        <v>128</v>
+      </c>
+      <c r="D20" s="1">
+        <v>805.88210000000004</v>
       </c>
       <c r="E20" s="1">
-        <v>256</v>
-      </c>
-      <c r="F20" s="6">
-        <v>3.0783377999999999</v>
+        <v>128</v>
+      </c>
+      <c r="F20" s="1">
+        <v>453.19540000000001</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="A21" s="1">
+        <v>256</v>
+      </c>
+      <c r="B21" s="1">
+        <v>23.964700000000001</v>
+      </c>
+      <c r="C21" s="1">
+        <v>256</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5217.6988000000001</v>
+      </c>
+      <c r="E21" s="1">
+        <v>256</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3105.5293000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>2</v>
-      </c>
-      <c r="B23" s="7">
-        <v>5.9000000000000003E-6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2</v>
-      </c>
-      <c r="D23" s="7">
-        <v>2.6800000000000001E-5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>2</v>
-      </c>
-      <c r="F23" s="7">
-        <v>2.1299999999999999E-5</v>
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7">
-        <v>1.11E-5</v>
+        <v>2</v>
+      </c>
+      <c r="B24" s="4">
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="C24" s="1">
-        <v>4</v>
-      </c>
-      <c r="D24" s="7">
-        <v>7.0699999999999997E-5</v>
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.46E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>4</v>
-      </c>
-      <c r="F24" s="7">
-        <v>1.496E-4</v>
+        <v>2</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1.8200000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>8</v>
-      </c>
-      <c r="B25" s="7">
-        <v>2.51E-5</v>
+        <v>4</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="C25" s="1">
-        <v>8</v>
-      </c>
-      <c r="D25" s="7">
-        <v>4.1439999999999999E-4</v>
+        <v>4</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>8</v>
-      </c>
-      <c r="F25" s="7">
-        <v>5.0310000000000003E-4</v>
+        <v>4</v>
+      </c>
+      <c r="F25" s="4">
+        <v>7.9799999999999996E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>16</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1.4449999999999999E-4</v>
+        <v>8</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="C26" s="1">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6">
-        <v>2.1251E-3</v>
+        <v>8</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.46150000000000002</v>
       </c>
       <c r="E26" s="1">
-        <v>16</v>
-      </c>
-      <c r="F26" s="6">
-        <v>1.9222E-3</v>
+        <v>8</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.54210000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>32</v>
-      </c>
-      <c r="B27" s="6">
-        <v>1.0502E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.13400000000000001</v>
       </c>
       <c r="C27" s="1">
-        <v>32</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1.1901500000000001E-2</v>
+        <v>16</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1.9690000000000001</v>
       </c>
       <c r="E27" s="1">
-        <v>32</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1.1963100000000001E-2</v>
+        <v>16</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1.9432</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>64</v>
-      </c>
-      <c r="B28" s="6">
-        <v>2.5390999999999999E-3</v>
+        <v>32</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1.0521</v>
       </c>
       <c r="C28" s="1">
-        <v>64</v>
-      </c>
-      <c r="D28" s="6">
-        <v>8.9461700000000005E-2</v>
+        <v>32</v>
+      </c>
+      <c r="D28" s="3">
+        <v>11.9229</v>
       </c>
       <c r="E28" s="1">
-        <v>64</v>
-      </c>
-      <c r="F28" s="6">
-        <v>8.0498600000000003E-2</v>
+        <v>32</v>
+      </c>
+      <c r="F28" s="3">
+        <v>13.0075</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>128</v>
-      </c>
-      <c r="B29" s="6">
-        <v>1.0145100000000001E-2</v>
+        <v>64</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2.5899000000000001</v>
       </c>
       <c r="C29" s="1">
-        <v>128</v>
-      </c>
-      <c r="D29" s="6">
-        <v>0.79149409999999998</v>
+        <v>64</v>
+      </c>
+      <c r="D29" s="3">
+        <v>90.809600000000003</v>
       </c>
       <c r="E29" s="1">
-        <v>128</v>
-      </c>
-      <c r="F29" s="6">
-        <v>0.4472836</v>
+        <v>64</v>
+      </c>
+      <c r="F29" s="3">
+        <v>81.313299999999998</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
+        <v>128</v>
+      </c>
+      <c r="B30" s="3">
+        <v>7.6612</v>
+      </c>
+      <c r="C30" s="1">
+        <v>128</v>
+      </c>
+      <c r="D30" s="3">
+        <v>798.23540000000003</v>
+      </c>
+      <c r="E30" s="1">
+        <v>128</v>
+      </c>
+      <c r="F30" s="3">
+        <v>450.19869999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>256</v>
       </c>
-      <c r="B30" s="6">
-        <v>2.3506300000000001E-2</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="B31" s="3">
+        <v>22.7835</v>
+      </c>
+      <c r="C31" s="1">
         <v>256</v>
       </c>
-      <c r="D30" s="6">
-        <v>5.2030342000000003</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D31" s="3">
+        <v>5328.4354000000003</v>
+      </c>
+      <c r="E31" s="1">
         <v>256</v>
       </c>
-      <c r="F30" s="6">
-        <v>3.1173041000000001</v>
+      <c r="F31" s="3">
+        <v>3145.2006999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2</v>
+      </c>
+      <c r="B34" s="4">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2.18E-2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>4</v>
+      </c>
+      <c r="B35" s="4">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="4">
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>4</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0.10680000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>8</v>
+      </c>
+      <c r="B36" s="4">
+        <v>2.06E-2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>8</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.48820000000000002</v>
+      </c>
+      <c r="E36" s="1">
+        <v>8</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.48430000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>16</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="C37" s="1">
+        <v>16</v>
+      </c>
+      <c r="D37" s="3">
+        <v>2.988</v>
+      </c>
+      <c r="E37" s="1">
+        <v>16</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2.0676000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>32</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.88360000000000005</v>
+      </c>
+      <c r="C38" s="1">
+        <v>32</v>
+      </c>
+      <c r="D38" s="3">
+        <v>12.6097</v>
+      </c>
+      <c r="E38" s="1">
+        <v>32</v>
+      </c>
+      <c r="F38" s="3">
+        <v>11.780900000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>64</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2.7109999999999999</v>
+      </c>
+      <c r="C39" s="1">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3">
+        <v>91.072500000000005</v>
+      </c>
+      <c r="E39" s="1">
+        <v>64</v>
+      </c>
+      <c r="F39" s="3">
+        <v>79.873999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>128</v>
+      </c>
+      <c r="B40" s="3">
+        <v>9.3246000000000002</v>
+      </c>
+      <c r="C40" s="1">
+        <v>128</v>
+      </c>
+      <c r="D40" s="3">
+        <v>783.64670000000001</v>
+      </c>
+      <c r="E40" s="1">
+        <v>128</v>
+      </c>
+      <c r="F40" s="3">
+        <v>453.96510000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>256</v>
+      </c>
+      <c r="B41" s="3">
+        <v>22.790500000000002</v>
+      </c>
+      <c r="C41" s="1">
+        <v>256</v>
+      </c>
+      <c r="D41" s="3">
+        <v>5261.1722</v>
+      </c>
+      <c r="E41" s="1">
+        <v>256</v>
+      </c>
+      <c r="F41" s="3">
+        <v>3123.2516999999998</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A21:F21"/>
+  <mergeCells count="7">
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A22:F22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>